<commit_message>
Fixed bug in empty player algorithm and added .mov support added 7 player support
</commit_message>
<xml_diff>
--- a/Output_Results/Tournament_Results.xlsx
+++ b/Output_Results/Tournament_Results.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -583,7 +583,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -628,7 +628,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -673,7 +673,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -718,7 +718,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -763,7 +763,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -808,7 +808,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -853,7 +853,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -898,7 +898,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -943,7 +943,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -988,7 +988,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Demo</t>
+          <t>Demo_CaptureCard_Race</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>